<commit_message>
KPC PEN dan MDM
</commit_message>
<xml_diff>
--- a/DB.xlsx
+++ b/DB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\github\kamusjsc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5012EA4-C401-4694-AD6B-79944A87CAA9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{290B33FF-674D-414D-9B1D-C38C2D44FBA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="807" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="817" uniqueCount="329">
   <si>
     <t>Singkatan</t>
   </si>
@@ -1003,6 +1003,18 @@
   </si>
   <si>
     <t>Bimbingan Teknis</t>
+  </si>
+  <si>
+    <t>Master Data Management</t>
+  </si>
+  <si>
+    <t>MDM</t>
+  </si>
+  <si>
+    <t>Komite Pengendalian Covid-19 dan Pemulihan Ekonomi Nasional</t>
+  </si>
+  <si>
+    <t>KPC PEN</t>
   </si>
 </sst>
 </file>
@@ -1324,10 +1336,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E162"/>
+  <dimension ref="A1:E164"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="F86" sqref="F86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2780,13 +2792,13 @@
         <v>316</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>12</v>
+        <v>328</v>
       </c>
       <c r="C86" s="2" t="s">
         <v>314</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>4</v>
+        <v>327</v>
       </c>
       <c r="E86" s="2" t="s">
         <v>315</v>
@@ -2797,13 +2809,13 @@
         <v>316</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>93</v>
+        <v>12</v>
       </c>
       <c r="C87" s="2" t="s">
         <v>314</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>94</v>
+        <v>4</v>
       </c>
       <c r="E87" s="2" t="s">
         <v>315</v>
@@ -2814,13 +2826,13 @@
         <v>316</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>121</v>
+        <v>326</v>
       </c>
       <c r="C88" s="2" t="s">
         <v>314</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>122</v>
+        <v>325</v>
       </c>
       <c r="E88" s="2" t="s">
         <v>315</v>
@@ -2831,13 +2843,13 @@
         <v>316</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C89" s="2" t="s">
         <v>314</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E89" s="2" t="s">
         <v>315</v>
@@ -2848,13 +2860,13 @@
         <v>316</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>170</v>
+        <v>121</v>
       </c>
       <c r="C90" s="2" t="s">
         <v>314</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>169</v>
+        <v>122</v>
       </c>
       <c r="E90" s="2" t="s">
         <v>315</v>
@@ -2865,13 +2877,13 @@
         <v>316</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>159</v>
+        <v>95</v>
       </c>
       <c r="C91" s="2" t="s">
         <v>314</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>160</v>
+        <v>96</v>
       </c>
       <c r="E91" s="2" t="s">
         <v>315</v>
@@ -2882,13 +2894,13 @@
         <v>316</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>73</v>
+        <v>170</v>
       </c>
       <c r="C92" s="2" t="s">
         <v>314</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>74</v>
+        <v>169</v>
       </c>
       <c r="E92" s="2" t="s">
         <v>315</v>
@@ -2899,13 +2911,13 @@
         <v>316</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>53</v>
+        <v>159</v>
       </c>
       <c r="C93" s="2" t="s">
         <v>314</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>54</v>
+        <v>160</v>
       </c>
       <c r="E93" s="2" t="s">
         <v>315</v>
@@ -2916,13 +2928,13 @@
         <v>316</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>230</v>
+        <v>73</v>
       </c>
       <c r="C94" s="2" t="s">
         <v>314</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>229</v>
+        <v>74</v>
       </c>
       <c r="E94" s="2" t="s">
         <v>315</v>
@@ -2933,13 +2945,13 @@
         <v>316</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>216</v>
+        <v>53</v>
       </c>
       <c r="C95" s="2" t="s">
         <v>314</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>231</v>
+        <v>54</v>
       </c>
       <c r="E95" s="2" t="s">
         <v>315</v>
@@ -2950,13 +2962,13 @@
         <v>316</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>26</v>
+        <v>230</v>
       </c>
       <c r="C96" s="2" t="s">
         <v>314</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>27</v>
+        <v>229</v>
       </c>
       <c r="E96" s="2" t="s">
         <v>315</v>
@@ -2967,13 +2979,13 @@
         <v>316</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>55</v>
+        <v>216</v>
       </c>
       <c r="C97" s="2" t="s">
         <v>314</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>56</v>
+        <v>231</v>
       </c>
       <c r="E97" s="2" t="s">
         <v>315</v>
@@ -2984,13 +2996,13 @@
         <v>316</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>219</v>
+        <v>26</v>
       </c>
       <c r="C98" s="2" t="s">
         <v>314</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>220</v>
+        <v>27</v>
       </c>
       <c r="E98" s="2" t="s">
         <v>315</v>
@@ -3001,13 +3013,13 @@
         <v>316</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>83</v>
+        <v>55</v>
       </c>
       <c r="C99" s="2" t="s">
         <v>314</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>84</v>
+        <v>56</v>
       </c>
       <c r="E99" s="2" t="s">
         <v>315</v>
@@ -3018,13 +3030,13 @@
         <v>316</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>321</v>
+        <v>219</v>
       </c>
       <c r="C100" s="2" t="s">
         <v>314</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>322</v>
+        <v>220</v>
       </c>
       <c r="E100" s="2" t="s">
         <v>315</v>
@@ -3035,13 +3047,13 @@
         <v>316</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>203</v>
+        <v>83</v>
       </c>
       <c r="C101" s="2" t="s">
         <v>314</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>204</v>
+        <v>84</v>
       </c>
       <c r="E101" s="2" t="s">
         <v>315</v>
@@ -3052,13 +3064,13 @@
         <v>316</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>201</v>
+        <v>321</v>
       </c>
       <c r="C102" s="2" t="s">
         <v>314</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>202</v>
+        <v>322</v>
       </c>
       <c r="E102" s="2" t="s">
         <v>315</v>
@@ -3069,13 +3081,13 @@
         <v>316</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>186</v>
+        <v>203</v>
       </c>
       <c r="C103" s="2" t="s">
         <v>314</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>187</v>
+        <v>204</v>
       </c>
       <c r="E103" s="2" t="s">
         <v>315</v>
@@ -3086,13 +3098,13 @@
         <v>316</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>238</v>
+        <v>201</v>
       </c>
       <c r="C104" s="2" t="s">
         <v>314</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>239</v>
+        <v>202</v>
       </c>
       <c r="E104" s="2" t="s">
         <v>315</v>
@@ -3103,13 +3115,13 @@
         <v>316</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>222</v>
+        <v>186</v>
       </c>
       <c r="C105" s="2" t="s">
         <v>314</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>221</v>
+        <v>187</v>
       </c>
       <c r="E105" s="2" t="s">
         <v>315</v>
@@ -3120,13 +3132,13 @@
         <v>316</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>144</v>
+        <v>238</v>
       </c>
       <c r="C106" s="2" t="s">
         <v>314</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>179</v>
+        <v>239</v>
       </c>
       <c r="E106" s="2" t="s">
         <v>315</v>
@@ -3137,13 +3149,13 @@
         <v>316</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>250</v>
+        <v>222</v>
       </c>
       <c r="C107" s="2" t="s">
         <v>314</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>251</v>
+        <v>221</v>
       </c>
       <c r="E107" s="2" t="s">
         <v>315</v>
@@ -3153,14 +3165,14 @@
       <c r="A108" t="s">
         <v>316</v>
       </c>
-      <c r="B108" t="s">
-        <v>258</v>
+      <c r="B108" s="2" t="s">
+        <v>144</v>
       </c>
       <c r="C108" s="2" t="s">
         <v>314</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>259</v>
+        <v>179</v>
       </c>
       <c r="E108" s="2" t="s">
         <v>315</v>
@@ -3171,13 +3183,13 @@
         <v>316</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>44</v>
+        <v>250</v>
       </c>
       <c r="C109" s="2" t="s">
         <v>314</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>43</v>
+        <v>251</v>
       </c>
       <c r="E109" s="2" t="s">
         <v>315</v>
@@ -3187,14 +3199,14 @@
       <c r="A110" t="s">
         <v>316</v>
       </c>
-      <c r="B110" s="2" t="s">
-        <v>149</v>
+      <c r="B110" t="s">
+        <v>258</v>
       </c>
       <c r="C110" s="2" t="s">
         <v>314</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>150</v>
+        <v>259</v>
       </c>
       <c r="E110" s="2" t="s">
         <v>315</v>
@@ -3205,13 +3217,13 @@
         <v>316</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>163</v>
+        <v>44</v>
       </c>
       <c r="C111" s="2" t="s">
         <v>314</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>164</v>
+        <v>43</v>
       </c>
       <c r="E111" s="2" t="s">
         <v>315</v>
@@ -3222,13 +3234,13 @@
         <v>316</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>289</v>
+        <v>149</v>
       </c>
       <c r="C112" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="D112" t="s">
-        <v>288</v>
+      <c r="D112" s="2" t="s">
+        <v>150</v>
       </c>
       <c r="E112" s="2" t="s">
         <v>315</v>
@@ -3239,13 +3251,13 @@
         <v>316</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>286</v>
+        <v>163</v>
       </c>
       <c r="C113" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="D113" t="s">
-        <v>287</v>
+      <c r="D113" s="2" t="s">
+        <v>164</v>
       </c>
       <c r="E113" s="2" t="s">
         <v>315</v>
@@ -3256,13 +3268,13 @@
         <v>316</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>161</v>
+        <v>289</v>
       </c>
       <c r="C114" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="D114" s="2" t="s">
-        <v>162</v>
+      <c r="D114" t="s">
+        <v>288</v>
       </c>
       <c r="E114" s="2" t="s">
         <v>315</v>
@@ -3273,13 +3285,13 @@
         <v>316</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>155</v>
+        <v>286</v>
       </c>
       <c r="C115" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="D115" s="2" t="s">
-        <v>156</v>
+      <c r="D115" t="s">
+        <v>287</v>
       </c>
       <c r="E115" s="2" t="s">
         <v>315</v>
@@ -3290,13 +3302,13 @@
         <v>316</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>113</v>
+        <v>161</v>
       </c>
       <c r="C116" s="2" t="s">
         <v>314</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>114</v>
+        <v>162</v>
       </c>
       <c r="E116" s="2" t="s">
         <v>315</v>
@@ -3307,13 +3319,13 @@
         <v>316</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>24</v>
+        <v>155</v>
       </c>
       <c r="C117" s="2" t="s">
         <v>314</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>25</v>
+        <v>156</v>
       </c>
       <c r="E117" s="2" t="s">
         <v>315</v>
@@ -3324,13 +3336,13 @@
         <v>316</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C118" s="2" t="s">
         <v>314</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="E118" s="2" t="s">
         <v>315</v>
@@ -3341,13 +3353,13 @@
         <v>316</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>157</v>
+        <v>24</v>
       </c>
       <c r="C119" s="2" t="s">
         <v>314</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>158</v>
+        <v>25</v>
       </c>
       <c r="E119" s="2" t="s">
         <v>315</v>
@@ -3357,14 +3369,14 @@
       <c r="A120" t="s">
         <v>316</v>
       </c>
-      <c r="B120" t="s">
-        <v>272</v>
+      <c r="B120" s="2" t="s">
+        <v>111</v>
       </c>
       <c r="C120" s="2" t="s">
         <v>314</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>273</v>
+        <v>112</v>
       </c>
       <c r="E120" s="2" t="s">
         <v>315</v>
@@ -3374,14 +3386,14 @@
       <c r="A121" t="s">
         <v>316</v>
       </c>
-      <c r="B121" t="s">
-        <v>270</v>
+      <c r="B121" s="2" t="s">
+        <v>157</v>
       </c>
       <c r="C121" s="2" t="s">
         <v>314</v>
       </c>
       <c r="D121" s="2" t="s">
-        <v>271</v>
+        <v>158</v>
       </c>
       <c r="E121" s="2" t="s">
         <v>315</v>
@@ -3391,14 +3403,14 @@
       <c r="A122" t="s">
         <v>316</v>
       </c>
-      <c r="B122" s="2" t="s">
-        <v>5</v>
+      <c r="B122" t="s">
+        <v>272</v>
       </c>
       <c r="C122" s="2" t="s">
         <v>314</v>
       </c>
       <c r="D122" s="2" t="s">
-        <v>6</v>
+        <v>273</v>
       </c>
       <c r="E122" s="2" t="s">
         <v>315</v>
@@ -3408,14 +3420,14 @@
       <c r="A123" t="s">
         <v>316</v>
       </c>
-      <c r="B123" s="2" t="s">
-        <v>306</v>
+      <c r="B123" t="s">
+        <v>270</v>
       </c>
       <c r="C123" s="2" t="s">
         <v>314</v>
       </c>
       <c r="D123" s="2" t="s">
-        <v>307</v>
+        <v>271</v>
       </c>
       <c r="E123" s="2" t="s">
         <v>315</v>
@@ -3426,13 +3438,13 @@
         <v>316</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>136</v>
+        <v>5</v>
       </c>
       <c r="C124" s="2" t="s">
         <v>314</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>137</v>
+        <v>6</v>
       </c>
       <c r="E124" s="2" t="s">
         <v>315</v>
@@ -3443,13 +3455,13 @@
         <v>316</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>29</v>
+        <v>306</v>
       </c>
       <c r="C125" s="2" t="s">
         <v>314</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>31</v>
+        <v>307</v>
       </c>
       <c r="E125" s="2" t="s">
         <v>315</v>
@@ -3460,13 +3472,13 @@
         <v>316</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>28</v>
+        <v>136</v>
       </c>
       <c r="C126" s="2" t="s">
         <v>314</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>30</v>
+        <v>137</v>
       </c>
       <c r="E126" s="2" t="s">
         <v>315</v>
@@ -3477,13 +3489,13 @@
         <v>316</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>227</v>
+        <v>29</v>
       </c>
       <c r="C127" s="2" t="s">
         <v>314</v>
       </c>
       <c r="D127" s="2" t="s">
-        <v>228</v>
+        <v>31</v>
       </c>
       <c r="E127" s="2" t="s">
         <v>315</v>
@@ -3494,13 +3506,13 @@
         <v>316</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>61</v>
+        <v>28</v>
       </c>
       <c r="C128" s="2" t="s">
         <v>314</v>
       </c>
       <c r="D128" s="2" t="s">
-        <v>62</v>
+        <v>30</v>
       </c>
       <c r="E128" s="2" t="s">
         <v>315</v>
@@ -3511,13 +3523,13 @@
         <v>316</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>153</v>
+        <v>227</v>
       </c>
       <c r="C129" s="2" t="s">
         <v>314</v>
       </c>
       <c r="D129" s="2" t="s">
-        <v>154</v>
+        <v>228</v>
       </c>
       <c r="E129" s="2" t="s">
         <v>315</v>
@@ -3528,13 +3540,13 @@
         <v>316</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C130" s="2" t="s">
         <v>314</v>
       </c>
       <c r="D130" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E130" s="2" t="s">
         <v>315</v>
@@ -3545,13 +3557,13 @@
         <v>316</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>91</v>
+        <v>153</v>
       </c>
       <c r="C131" s="2" t="s">
         <v>314</v>
       </c>
       <c r="D131" s="2" t="s">
-        <v>92</v>
+        <v>154</v>
       </c>
       <c r="E131" s="2" t="s">
         <v>315</v>
@@ -3561,14 +3573,14 @@
       <c r="A132" t="s">
         <v>316</v>
       </c>
-      <c r="B132" t="s">
-        <v>254</v>
+      <c r="B132" s="2" t="s">
+        <v>59</v>
       </c>
       <c r="C132" s="2" t="s">
         <v>314</v>
       </c>
       <c r="D132" s="2" t="s">
-        <v>255</v>
+        <v>60</v>
       </c>
       <c r="E132" s="2" t="s">
         <v>315</v>
@@ -3579,13 +3591,13 @@
         <v>316</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>217</v>
+        <v>91</v>
       </c>
       <c r="C133" s="2" t="s">
         <v>314</v>
       </c>
       <c r="D133" s="2" t="s">
-        <v>218</v>
+        <v>92</v>
       </c>
       <c r="E133" s="2" t="s">
         <v>315</v>
@@ -3595,14 +3607,14 @@
       <c r="A134" t="s">
         <v>316</v>
       </c>
-      <c r="B134" s="2" t="s">
-        <v>51</v>
+      <c r="B134" t="s">
+        <v>254</v>
       </c>
       <c r="C134" s="2" t="s">
         <v>314</v>
       </c>
       <c r="D134" s="2" t="s">
-        <v>52</v>
+        <v>255</v>
       </c>
       <c r="E134" s="2" t="s">
         <v>315</v>
@@ -3613,13 +3625,13 @@
         <v>316</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>123</v>
+        <v>217</v>
       </c>
       <c r="C135" s="2" t="s">
         <v>314</v>
       </c>
       <c r="D135" s="2" t="s">
-        <v>124</v>
+        <v>218</v>
       </c>
       <c r="E135" s="2" t="s">
         <v>315</v>
@@ -3630,13 +3642,13 @@
         <v>316</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>103</v>
+        <v>51</v>
       </c>
       <c r="C136" s="2" t="s">
         <v>314</v>
       </c>
       <c r="D136" s="2" t="s">
-        <v>104</v>
+        <v>52</v>
       </c>
       <c r="E136" s="2" t="s">
         <v>315</v>
@@ -3647,13 +3659,13 @@
         <v>316</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>16</v>
+        <v>123</v>
       </c>
       <c r="C137" s="2" t="s">
         <v>314</v>
       </c>
       <c r="D137" s="2" t="s">
-        <v>23</v>
+        <v>124</v>
       </c>
       <c r="E137" s="2" t="s">
         <v>315</v>
@@ -3664,13 +3676,13 @@
         <v>316</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>50</v>
+        <v>103</v>
       </c>
       <c r="C138" s="2" t="s">
         <v>314</v>
       </c>
       <c r="D138" s="2" t="s">
-        <v>49</v>
+        <v>104</v>
       </c>
       <c r="E138" s="2" t="s">
         <v>315</v>
@@ -3681,13 +3693,13 @@
         <v>316</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="C139" s="2" t="s">
         <v>314</v>
       </c>
       <c r="D139" s="2" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="E139" s="2" t="s">
         <v>315</v>
@@ -3698,13 +3710,13 @@
         <v>316</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="C140" s="2" t="s">
         <v>314</v>
       </c>
       <c r="D140" s="2" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="E140" s="2" t="s">
         <v>315</v>
@@ -3715,13 +3727,13 @@
         <v>316</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>294</v>
+        <v>37</v>
       </c>
       <c r="C141" s="2" t="s">
         <v>314</v>
       </c>
       <c r="D141" s="2" t="s">
-        <v>295</v>
+        <v>38</v>
       </c>
       <c r="E141" s="2" t="s">
         <v>315</v>
@@ -3732,13 +3744,13 @@
         <v>316</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>242</v>
+        <v>32</v>
       </c>
       <c r="C142" s="2" t="s">
         <v>314</v>
       </c>
       <c r="D142" s="2" t="s">
-        <v>243</v>
+        <v>34</v>
       </c>
       <c r="E142" s="2" t="s">
         <v>315</v>
@@ -3749,13 +3761,13 @@
         <v>316</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>304</v>
+        <v>294</v>
       </c>
       <c r="C143" s="2" t="s">
         <v>314</v>
       </c>
       <c r="D143" s="2" t="s">
-        <v>305</v>
+        <v>295</v>
       </c>
       <c r="E143" s="2" t="s">
         <v>315</v>
@@ -3766,13 +3778,13 @@
         <v>316</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>310</v>
+        <v>242</v>
       </c>
       <c r="C144" s="2" t="s">
         <v>314</v>
       </c>
       <c r="D144" s="2" t="s">
-        <v>311</v>
+        <v>243</v>
       </c>
       <c r="E144" s="2" t="s">
         <v>315</v>
@@ -3783,13 +3795,13 @@
         <v>316</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>105</v>
+        <v>304</v>
       </c>
       <c r="C145" s="2" t="s">
         <v>314</v>
       </c>
       <c r="D145" s="2" t="s">
-        <v>106</v>
+        <v>305</v>
       </c>
       <c r="E145" s="2" t="s">
         <v>315</v>
@@ -3800,13 +3812,13 @@
         <v>316</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>39</v>
+        <v>310</v>
       </c>
       <c r="C146" s="2" t="s">
         <v>314</v>
       </c>
       <c r="D146" s="2" t="s">
-        <v>40</v>
+        <v>311</v>
       </c>
       <c r="E146" s="2" t="s">
         <v>315</v>
@@ -3816,14 +3828,14 @@
       <c r="A147" t="s">
         <v>316</v>
       </c>
-      <c r="B147" t="s">
-        <v>274</v>
+      <c r="B147" s="2" t="s">
+        <v>105</v>
       </c>
       <c r="C147" s="2" t="s">
         <v>314</v>
       </c>
       <c r="D147" s="2" t="s">
-        <v>275</v>
+        <v>106</v>
       </c>
       <c r="E147" s="2" t="s">
         <v>315</v>
@@ -3834,13 +3846,13 @@
         <v>316</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>142</v>
+        <v>39</v>
       </c>
       <c r="C148" s="2" t="s">
         <v>314</v>
       </c>
       <c r="D148" s="2" t="s">
-        <v>143</v>
+        <v>40</v>
       </c>
       <c r="E148" s="2" t="s">
         <v>315</v>
@@ -3850,14 +3862,14 @@
       <c r="A149" t="s">
         <v>316</v>
       </c>
-      <c r="B149" s="2" t="s">
-        <v>142</v>
+      <c r="B149" t="s">
+        <v>274</v>
       </c>
       <c r="C149" s="2" t="s">
         <v>314</v>
       </c>
       <c r="D149" s="2" t="s">
-        <v>200</v>
+        <v>275</v>
       </c>
       <c r="E149" s="2" t="s">
         <v>315</v>
@@ -3868,13 +3880,13 @@
         <v>316</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="C150" s="2" t="s">
         <v>314</v>
       </c>
       <c r="D150" s="2" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="E150" s="2" t="s">
         <v>315</v>
@@ -3885,13 +3897,13 @@
         <v>316</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>296</v>
+        <v>142</v>
       </c>
       <c r="C151" s="2" t="s">
         <v>314</v>
       </c>
       <c r="D151" s="2" t="s">
-        <v>297</v>
+        <v>200</v>
       </c>
       <c r="E151" s="2" t="s">
         <v>315</v>
@@ -3902,13 +3914,13 @@
         <v>316</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>115</v>
+        <v>138</v>
       </c>
       <c r="C152" s="2" t="s">
         <v>314</v>
       </c>
       <c r="D152" s="2" t="s">
-        <v>116</v>
+        <v>139</v>
       </c>
       <c r="E152" s="2" t="s">
         <v>315</v>
@@ -3919,13 +3931,13 @@
         <v>316</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>308</v>
+        <v>296</v>
       </c>
       <c r="C153" s="2" t="s">
         <v>314</v>
       </c>
       <c r="D153" s="2" t="s">
-        <v>309</v>
+        <v>297</v>
       </c>
       <c r="E153" s="2" t="s">
         <v>315</v>
@@ -3936,13 +3948,13 @@
         <v>316</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>223</v>
+        <v>115</v>
       </c>
       <c r="C154" s="2" t="s">
         <v>314</v>
       </c>
       <c r="D154" s="2" t="s">
-        <v>224</v>
+        <v>116</v>
       </c>
       <c r="E154" s="2" t="s">
         <v>315</v>
@@ -3953,13 +3965,13 @@
         <v>316</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>131</v>
+        <v>308</v>
       </c>
       <c r="C155" s="2" t="s">
         <v>314</v>
       </c>
       <c r="D155" s="2" t="s">
-        <v>132</v>
+        <v>309</v>
       </c>
       <c r="E155" s="2" t="s">
         <v>315</v>
@@ -3970,13 +3982,13 @@
         <v>316</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>65</v>
+        <v>223</v>
       </c>
       <c r="C156" s="2" t="s">
         <v>314</v>
       </c>
       <c r="D156" s="2" t="s">
-        <v>66</v>
+        <v>224</v>
       </c>
       <c r="E156" s="2" t="s">
         <v>315</v>
@@ -3987,13 +3999,13 @@
         <v>316</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>107</v>
+        <v>131</v>
       </c>
       <c r="C157" s="2" t="s">
         <v>314</v>
       </c>
       <c r="D157" s="2" t="s">
-        <v>108</v>
+        <v>132</v>
       </c>
       <c r="E157" s="2" t="s">
         <v>315</v>
@@ -4004,13 +4016,13 @@
         <v>316</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>109</v>
+        <v>65</v>
       </c>
       <c r="C158" s="2" t="s">
         <v>314</v>
       </c>
       <c r="D158" s="2" t="s">
-        <v>110</v>
+        <v>66</v>
       </c>
       <c r="E158" s="2" t="s">
         <v>315</v>
@@ -4021,13 +4033,13 @@
         <v>316</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>167</v>
+        <v>107</v>
       </c>
       <c r="C159" s="2" t="s">
         <v>314</v>
       </c>
       <c r="D159" s="2" t="s">
-        <v>168</v>
+        <v>108</v>
       </c>
       <c r="E159" s="2" t="s">
         <v>315</v>
@@ -4038,13 +4050,13 @@
         <v>316</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
       <c r="C160" s="2" t="s">
         <v>314</v>
       </c>
       <c r="D160" s="2" t="s">
-        <v>98</v>
+        <v>110</v>
       </c>
       <c r="E160" s="2" t="s">
         <v>315</v>
@@ -4055,13 +4067,13 @@
         <v>316</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="C161" s="2" t="s">
         <v>314</v>
       </c>
       <c r="D161" s="2" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="E161" s="2" t="s">
         <v>315</v>
@@ -4072,15 +4084,49 @@
         <v>316</v>
       </c>
       <c r="B162" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C162" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="D162" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E162" s="2" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A163" t="s">
+        <v>316</v>
+      </c>
+      <c r="B163" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C163" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="D163" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="E163" s="2" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A164" t="s">
+        <v>316</v>
+      </c>
+      <c r="B164" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="C162" s="2" t="s">
-        <v>314</v>
-      </c>
-      <c r="D162" s="2" t="s">
+      <c r="C164" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="D164" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="E162" s="2" t="s">
+      <c r="E164" s="2" t="s">
         <v>315</v>
       </c>
     </row>

</xml_diff>